<commit_message>
Suppression 1 alerte + modif alerts
</commit_message>
<xml_diff>
--- a/220728_Plannings_expé_signal_d_alerte_CdB___Echappée.xlsx
+++ b/220728_Plannings_expé_signal_d_alerte_CdB___Echappée.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/brice_petit_ulb_be/Documents/Ulb/PhD/benevolat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/brice_petit_ulb_be/Documents/Ulb/PhD/VdE/VdE_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_453C11E74CDCB05EA9D989C5B408936919EB172D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{96E34AD2-AFC7-4FBA-A8BB-A0961BA8A6B8}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_453C11E74CDCB05EA9D989C5B408936919EB172D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DAF9337F-5327-46CB-AF8F-F84DC704CA75}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning expé" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="27">
   <si>
     <t>Planning expérimentation "signal d'alerte" Coin du Balai + Echappée</t>
   </si>
@@ -654,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,145 +928,134 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="9">
-        <v>44836</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="13">
+        <v>44843</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="9">
+        <v>44844</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="13">
-        <v>44843</v>
-      </c>
-      <c r="C26" s="8" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="13">
+        <v>44853</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="9">
+        <v>44863</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="13">
+        <v>44870</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="9">
+        <v>44874</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="13">
+        <v>44880</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="9">
+        <v>44889</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="13">
+        <v>44899</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="9">
-        <v>44844</v>
-      </c>
-      <c r="C27" s="4" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="9">
+        <v>44901</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="13">
-        <v>44853</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="9">
-        <v>44863</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="13">
-        <v>44870</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="9">
-        <v>44874</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="13">
-        <v>44880</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="9">
-        <v>44889</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="13">
-        <v>44899</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="9">
-        <v>44901</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>9</v>
+      <c r="A35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="13">
+        <v>44914</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="13">
-        <v>44914</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="9">
+      <c r="A36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="9">
         <v>44917</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1080,12 +1069,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37c45c7d-ab5f-44bc-a5e0-e5761a896314">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="cc187c68-baab-4236-9dad-d06e77fa50de" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1278,20 +1269,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37c45c7d-ab5f-44bc-a5e0-e5761a896314">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="cc187c68-baab-4236-9dad-d06e77fa50de" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CF9D036-0713-4B79-81DF-2FB8ED7C4D26}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA3BCDE7-4E5B-47E2-8163-201B8FF8D937}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="37c45c7d-ab5f-44bc-a5e0-e5761a896314"/>
+    <ds:schemaRef ds:uri="cc187c68-baab-4236-9dad-d06e77fa50de"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1316,12 +1308,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA3BCDE7-4E5B-47E2-8163-201B8FF8D937}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CF9D036-0713-4B79-81DF-2FB8ED7C4D26}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="37c45c7d-ab5f-44bc-a5e0-e5761a896314"/>
-    <ds:schemaRef ds:uri="cc187c68-baab-4236-9dad-d06e77fa50de"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>